<commit_message>
update db with animal type and size
</commit_message>
<xml_diff>
--- a/db/dicc_gps.xlsx
+++ b/db/dicc_gps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajpelu/SERPAM Dropbox/antonioj perezluque/vreGI/vreGI_db/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3560D8-606B-A047-9D38-506ACE76AD7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CE6D9C-49E3-A349-8C31-A1FA75053395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="28800" windowHeight="16380" activeTab="2" xr2:uid="{D072D900-3A35-0847-B582-0DCF0F9D656E}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="28800" windowHeight="18100" activeTab="1" xr2:uid="{D072D900-3A35-0847-B582-0DCF0F9D656E}"/>
   </bookViews>
   <sheets>
     <sheet name="dicc_ganaderos" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="168">
   <si>
     <t>user_name</t>
   </si>
@@ -518,13 +518,34 @@
   </si>
   <si>
     <t>GPS_14</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>obs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the number is for all herds of this sheperd </t>
+  </si>
+  <si>
+    <t>animal</t>
+  </si>
+  <si>
+    <t>oveja</t>
+  </si>
+  <si>
+    <t>cabra | oveja</t>
+  </si>
+  <si>
+    <t>cabra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -552,6 +573,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -573,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -585,6 +613,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1096,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0500B323-49C9-3443-BF24-D23965D728E9}">
   <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H94" sqref="H94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1105,9 +1137,10 @@
     <col min="3" max="3" width="18.83203125" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
     <col min="5" max="5" width="31.5" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -1123,8 +1156,11 @@
       <c r="E1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1140,8 +1176,11 @@
       <c r="E2" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1157,8 +1196,11 @@
       <c r="E3" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1174,8 +1216,11 @@
       <c r="E4" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1191,8 +1236,11 @@
       <c r="E5" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1208,8 +1256,11 @@
       <c r="E6" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1225,8 +1276,11 @@
       <c r="E7" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1242,8 +1296,11 @@
       <c r="E8" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1259,8 +1316,11 @@
       <c r="E9" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1276,8 +1336,11 @@
       <c r="E10" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1293,8 +1356,11 @@
       <c r="E11" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1310,8 +1376,11 @@
       <c r="E12" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1327,8 +1396,11 @@
       <c r="E13" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1344,8 +1416,11 @@
       <c r="E14" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1361,8 +1436,11 @@
       <c r="E15" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1378,8 +1456,11 @@
       <c r="E16" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1395,8 +1476,11 @@
       <c r="E17" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1412,8 +1496,11 @@
       <c r="E18" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1429,8 +1516,11 @@
       <c r="E19" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1446,8 +1536,11 @@
       <c r="E20" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1463,8 +1556,11 @@
       <c r="E21" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1480,8 +1576,11 @@
       <c r="E22" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1497,8 +1596,11 @@
       <c r="E23" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1514,8 +1616,11 @@
       <c r="E24" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1531,8 +1636,11 @@
       <c r="E25" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1548,8 +1656,11 @@
       <c r="E26" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1565,8 +1676,11 @@
       <c r="E27" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1582,8 +1696,11 @@
       <c r="E28" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1599,8 +1716,11 @@
       <c r="E29" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1616,8 +1736,11 @@
       <c r="E30" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1633,8 +1756,11 @@
       <c r="E31" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1650,8 +1776,11 @@
       <c r="E32" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1668,7 +1797,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1685,7 +1814,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1702,7 +1831,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1718,8 +1847,11 @@
       <c r="E36" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1735,8 +1867,11 @@
       <c r="E37" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1752,8 +1887,11 @@
       <c r="E38" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1769,8 +1907,11 @@
       <c r="E39" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1786,8 +1927,11 @@
       <c r="E40" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1803,8 +1947,11 @@
       <c r="E41" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1820,8 +1967,11 @@
       <c r="E42" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1837,8 +1987,11 @@
       <c r="E43" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1854,8 +2007,11 @@
       <c r="E44" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1871,8 +2027,11 @@
       <c r="E45" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1888,8 +2047,11 @@
       <c r="E46" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1905,8 +2067,11 @@
       <c r="E47" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1922,8 +2087,11 @@
       <c r="E48" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1939,8 +2107,11 @@
       <c r="E49" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1956,8 +2127,11 @@
       <c r="E50" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1973,8 +2147,11 @@
       <c r="E51" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1990,8 +2167,11 @@
       <c r="E52" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2007,8 +2187,11 @@
       <c r="E53" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2024,8 +2207,11 @@
       <c r="E54" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2041,8 +2227,11 @@
       <c r="E55" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2058,8 +2247,11 @@
       <c r="E56" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2076,7 +2268,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2093,7 +2285,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2109,8 +2301,11 @@
       <c r="E59" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2126,8 +2321,11 @@
       <c r="E60" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2143,8 +2341,11 @@
       <c r="E61" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2160,8 +2361,11 @@
       <c r="E62" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2177,8 +2381,11 @@
       <c r="E63" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2194,8 +2401,11 @@
       <c r="E64" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2211,8 +2421,11 @@
       <c r="E65" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2228,8 +2441,11 @@
       <c r="E66" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2245,8 +2461,11 @@
       <c r="E67" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2262,8 +2481,11 @@
       <c r="E68" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2279,8 +2501,11 @@
       <c r="E69" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2296,8 +2521,11 @@
       <c r="E70" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2313,8 +2541,11 @@
       <c r="E71" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2330,8 +2561,11 @@
       <c r="E72" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2347,8 +2581,11 @@
       <c r="E73" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2364,8 +2601,11 @@
       <c r="E74" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2381,8 +2621,11 @@
       <c r="E75" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2398,8 +2641,11 @@
       <c r="E76" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2415,8 +2661,11 @@
       <c r="E77" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2432,8 +2681,11 @@
       <c r="E78" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2449,8 +2701,11 @@
       <c r="E79" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2465,6 +2720,9 @@
       </c>
       <c r="E80" s="1" t="s">
         <v>51</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
@@ -2483,6 +2741,9 @@
       <c r="E81" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="F81" s="6" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82">
@@ -2500,6 +2761,9 @@
       <c r="E82" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="F82" s="6" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83">
@@ -2517,6 +2781,9 @@
       <c r="E83" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="F83" s="6" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84">
@@ -2534,6 +2801,9 @@
       <c r="E84" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="F84" s="6" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85">
@@ -2551,6 +2821,9 @@
       <c r="E85" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="F85" s="6" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86">
@@ -2568,6 +2841,9 @@
       <c r="E86" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="F86" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87">
@@ -2585,6 +2861,9 @@
       <c r="E87" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="F87" t="s">
+        <v>165</v>
+      </c>
       <c r="I87" s="1"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
@@ -2603,6 +2882,9 @@
       <c r="E88" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="F88" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89">
@@ -2620,6 +2902,9 @@
       <c r="E89" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="F89" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90">
@@ -2637,6 +2922,9 @@
       <c r="E90" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="F90" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91">
@@ -2654,6 +2942,9 @@
       <c r="E91" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="F91" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92">
@@ -2671,6 +2962,9 @@
       <c r="E92" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="F92" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93">
@@ -2688,6 +2982,9 @@
       <c r="E93" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="F93" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94">
@@ -2705,6 +3002,9 @@
       <c r="E94" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="F94" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95">
@@ -2721,6 +3021,9 @@
       </c>
       <c r="E95" s="1" t="s">
         <v>50</v>
+      </c>
+      <c r="F95" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2731,10 +3034,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3E1F52-1F19-1D4C-B88C-969FFCAF115D}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" zoomScaleNormal="143" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView zoomScale="143" zoomScaleNormal="143" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2742,9 +3045,11 @@
     <col min="1" max="1" width="12.1640625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="5"/>
+    <col min="5" max="5" width="36.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -2754,56 +3059,80 @@
       <c r="C1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="5">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="5">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="5">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="5">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2813,8 +3142,14 @@
       <c r="C8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="5">
+        <v>600</v>
+      </c>
+      <c r="E8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2824,8 +3159,14 @@
       <c r="C9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" s="5">
+        <v>600</v>
+      </c>
+      <c r="E9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -2835,8 +3176,14 @@
       <c r="C10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" s="5">
+        <v>600</v>
+      </c>
+      <c r="E10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -2846,8 +3193,11 @@
       <c r="C11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" s="5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -2857,16 +3207,22 @@
       <c r="C12" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" s="5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" s="5">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -2876,8 +3232,11 @@
       <c r="C14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" s="5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -2887,8 +3246,14 @@
       <c r="C15" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E15" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -2898,8 +3263,14 @@
       <c r="C16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -2909,8 +3280,11 @@
       <c r="C17" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" s="5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
@@ -2920,8 +3294,14 @@
       <c r="C18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" s="5">
+        <v>500</v>
+      </c>
+      <c r="E18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
@@ -2930,6 +3310,12 @@
       </c>
       <c r="C19" t="s">
         <v>33</v>
+      </c>
+      <c r="D19" s="5">
+        <v>500</v>
+      </c>
+      <c r="E19" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>